<commit_message>
little change on the front-end
</commit_message>
<xml_diff>
--- a/twitter_backend/static/UserWordsofInterestV2.xlsx
+++ b/twitter_backend/static/UserWordsofInterestV2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0490894-F1F1-4BA0-BDA7-85F1B7138580}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E5E29A-D3A4-4CF3-BD57-ED2BB6327404}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>New South Wales</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Marriage made in Redfern. @ Redfern, New South Wales</t>
   </si>
   <si>
-    <t>Literally the cutest photo on the internet today!</t>
-  </si>
-  <si>
     <t>@britjfrain British coastline has been eroding at the rate of knots for years too. Same out here in Australia</t>
   </si>
   <si>
@@ -91,12 +88,6 @@
     <t>White Queen</t>
   </si>
   <si>
-    <t>Boorowa war memorial. @ Boorowa, New South Wales</t>
-  </si>
-  <si>
-    <t>Just your typical gum tree is a typical sunset @ Wombatz Retreat</t>
-  </si>
-  <si>
     <t>When coffee art comes alive and tries to escape. @ Cafe Cornerstone</t>
   </si>
   <si>
@@ -106,10 +97,19 @@
     <t>artwork</t>
   </si>
   <si>
-    <t>….really need this one???</t>
-  </si>
-  <si>
-    <t>???</t>
+    <t>@james_frain Loving James in this. He's making me giggle, which is plain wrong LOL</t>
+  </si>
+  <si>
+    <t>📷 Now if the wind changes… Hilarious photo found on Instagram.</t>
+  </si>
+  <si>
+    <t>Well we girls didn’t give up like the boys did. @ Wombatz Retreat</t>
+  </si>
+  <si>
+    <t>Toys galore. A not so typical house in Boorowa. @ Boorowa, New South Wales</t>
+  </si>
+  <si>
+    <t>@startrekcbs OMG Burnham. OMG Tyler. OMG Lorca. OMG L’rell. OMG Tilly. OMG Saru. OMG Georgiou. OMG Stamets. OMG Cul…</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -481,7 +481,7 @@
         <v>5491</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D2" s="7">
         <v>43153.450069444443</v>
@@ -495,7 +495,7 @@
         <v>6627</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4">
         <v>43179.535995370374</v>
@@ -506,7 +506,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>4489</v>
+        <v>8489</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
@@ -522,8 +522,8 @@
       <c r="B5" s="3">
         <v>5448</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" t="s">
+        <v>25</v>
       </c>
       <c r="D5" s="4">
         <v>43157.340671296297</v>
@@ -551,7 +551,7 @@
         <v>5472</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4">
         <v>43125.495578703703</v>
@@ -565,7 +565,7 @@
         <v>5824</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="4">
         <v>43146.96769675926</v>
@@ -607,7 +607,7 @@
         <v>9945</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D11" s="4">
         <v>43121.476087962961</v>
@@ -615,13 +615,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>3645</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D12" s="4">
         <v>43092.987881944442</v>
@@ -629,13 +629,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1">
         <v>4187</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="4">
         <v>43055.083599537036</v>
@@ -648,11 +648,11 @@
       <c r="B14" s="6">
         <v>3839</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" t="s">
         <v>29</v>
+      </c>
+      <c r="D14" s="4">
+        <v>43122.497442129628</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
@@ -663,7 +663,7 @@
         <v>4716</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="4">
         <v>43126.253495370373</v>

</xml_diff>